<commit_message>
Added a default constructor in PwEntry
</commit_message>
<xml_diff>
--- a/MergeList.xlsx
+++ b/MergeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\github\containers\KPCLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E984FA52-7BD7-4068-92CD-3C4D804AE287}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB22086-ABE0-43FC-A33C-285A71066ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="765" windowWidth="21600" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="3000" windowWidth="17640" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>CryptoRandom.cs</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Native/</t>
+  </si>
+  <si>
+    <t>PwEntry.cs</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,118 +555,123 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>10</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to KeePass 2.48.1
</commit_message>
<xml_diff>
--- a/MergeList.xlsx
+++ b/MergeList.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\github\containers\KPCLib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB22086-ABE0-43FC-A33C-285A71066ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="3000" windowWidth="17640" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="3000" windowWidth="17640" windowHeight="11856" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2.47-2.48.1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="56">
   <si>
     <t>CryptoRandom.cs</t>
   </si>
@@ -121,13 +116,85 @@
   </si>
   <si>
     <t>PwEntry.cs</t>
+  </si>
+  <si>
+    <t>KPCLib</t>
+  </si>
+  <si>
+    <t>2.48.1</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>ProtectedBinarySet.cs</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>Copied 2.48.1</t>
+  </si>
+  <si>
+    <t>StringDictionaryEx.cs</t>
+  </si>
+  <si>
+    <t>No action</t>
+  </si>
+  <si>
+    <t>CryptoUtil.cs</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>IStructureItem.cs</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ClipboardU.cs</t>
+  </si>
+  <si>
+    <t>KdbxFile.cs</t>
+  </si>
+  <si>
+    <t>KdbxFile.Read.cs</t>
+  </si>
+  <si>
+    <t>KdbxFile.Read.Streamed.cs</t>
+  </si>
+  <si>
+    <t>KdbxFile.Write.cs</t>
+  </si>
+  <si>
+    <t>MemUtil.cs</t>
+  </si>
+  <si>
+    <t>No trivial merge</t>
+  </si>
+  <si>
+    <t>PwDefs.cs</t>
+  </si>
+  <si>
+    <t>PwGroup.cs</t>
+  </si>
+  <si>
+    <t>PwGroup.Search.cs</t>
+  </si>
+  <si>
+    <t>PwUuid.cs</t>
+  </si>
+  <si>
+    <t>Need to check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +210,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -160,13 +235,267 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,24 +768,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,4 +1008,774 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="29">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="32">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="35">
+        <v>5</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="35">
+        <v>7</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>8</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>9</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>10</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>11</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="34"/>
+      <c r="B19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="35">
+        <v>12</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>13</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>14</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>15</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>16</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>17</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="34"/>
+      <c r="B27" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>18</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>19</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>20</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>21</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="34"/>
+      <c r="B32" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>22</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>23</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>24</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="25"/>
+      <c r="E35" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>25</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>26</v>
+      </c>
+      <c r="B37" s="25"/>
+      <c r="C37" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="35">
+        <v>27</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="26"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>28</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>29</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>30</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>31</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>32</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>33</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11">
+        <v>34</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>